<commit_message>
Resolving version conflicts in Excel documents (I hate merge conflicts).
</commit_message>
<xml_diff>
--- a/ExcelTemplates/BestBuy.xlsx
+++ b/ExcelTemplates/BestBuy.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
   <si>
     <t>Seller</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>http://www.bestbuy.ca/Search/SearchResults.aspx?</t>
+  </si>
+  <si>
+    <t>h4</t>
+  </si>
+  <si>
+    <t>prod-title</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -609,25 +615,31 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -635,24 +647,18 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
@@ -683,7 +689,7 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -699,7 +705,7 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -715,6 +721,38 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final(?) push of Excel templates for testing.
</commit_message>
<xml_diff>
--- a/ExcelTemplates/BestBuy.xlsx
+++ b/ExcelTemplates/BestBuy.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
   <si>
     <t>Seller</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>price-wrapper price-medium</t>
-  </si>
-  <si>
-    <t>prodprice</t>
   </si>
   <si>
     <t>span</t>
@@ -507,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -530,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -615,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -631,7 +628,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -720,9 +717,6 @@
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
@@ -737,7 +731,7 @@
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -753,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>